<commit_message>
datatypes instead of actual data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -18,66 +18,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>qwererqwe</t>
+    <t>CharField</t>
   </si>
   <si>
-    <t>asdfgssdkcsdj</t>
+    <t>TextField</t>
   </si>
   <si>
-    <t>sjosdocjd</t>
+    <t>PositiveIntegerField</t>
   </si>
   <si>
-    <t>dsjncoawnmdsnkmc,nsadiojc</t>
+    <t>IntegerField</t>
   </si>
   <si>
-    <t>oiiwjkwencnods</t>
-  </si>
-  <si>
-    <t>sdknacomwklmcqwmoecmao</t>
-  </si>
-  <si>
-    <t>ksdkfmsdkl</t>
-  </si>
-  <si>
-    <t>[{"_id":"5b20b297fc28b53b80bb588b","index":0,"guid":"b9cc2193-c475-4f86-9c5d-ba1c1eb17cfa","isActive":false,"balance":"$2,544.76","picture":"http://placehold.it/32x32","age":35,"eyeColor":"blue","name":"Deana Cohen"},{"_id":"5b20b2973f8a4a90ad8c35fc","index":1,"guid":"b2b0f4d5-39e1-4321-b300-3c08c0eacf4b","isActive":false,"balance":"$2,252.69","picture":"http://placehold.it/32x32","age":25,"eyeColor":"brown","name":"Chen Hooper"},{"_id":"5b20b2977df4355aa7b993af","index":2,"guid":"1f0c0829-f9ab-4eb6-b106-377e41086ddf","isActive":false,"balance":"$1,116.92","picture":"http://placehold.it/32x32","age":37,"eyeColor":"brown","name":"Arnold Wilson"},{"_id":"5b20b2973400739f91af8f3f","index":3,"guid":"14662d70-6e10-4d6b-bba8-24322fe79ad3","isActive":false,"balance":"$1,231.11","picture":"http://placehold.it/32x32","age":23,"eyeColor":"green","name":"Berta Clark"},{"_id":"5b20b297b9504bbe4b26303f","index":4,"guid":"966ec57f-f3ce-4eab-9d2f-636f3f1f89f1","isActive":true,"balance":"$1,310.59","picture":"http://placehold.it/32x32","age":35,"eyeColor":"brown","name":"Vaughn Ellison"},{"_id":"5b20b297f043757eca7cdedc","index":5,"guid":"22469496-b935-448a-b206-3fa34aa4341c","isActive":false,"balance":"$3,774.91","picture":"http://placehold.it/32x32","age":28,"eyeColor":"green","name":"Jacqueline Nixon"}]</t>
-  </si>
-  <si>
-    <t>jojojojo</t>
-  </si>
-  <si>
-    <t>dsaodam</t>
-  </si>
-  <si>
-    <t>[{"_id":"5b20b2e08eecb505d87866e3","index":0,"guid":"58bd755f-51a8-424f-99e8-e3220f3214fc","isActive":false,"balance":"$3,348.08","picture":"http://placehold.it/32x32","age":36,"eyeColor":"blue","name":"Lee Massey"},{"_id":"5b20b2e0cc83ce4eaecf4feb","index":1,"guid":"9e1d4a03-2d57-476e-813b-b9de771dd7e2","isActive":false,"balance":"$1,088.91","picture":"http://placehold.it/32x32","age":29,"eyeColor":"green","name":"Candice Barrera"},{"_id":"5b20b2e0422521d975c72380","index":2,"guid":"bd5e508f-b655-4916-a154-aac20685c32b","isActive":true,"balance":"$1,120.71","picture":"http://placehold.it/32x32","age":20,"eyeColor":"green","name":"Simon Meyers"},{"_id":"5b20b2e05f7d2e2e364d0829","index":3,"guid":"11f9e3d7-1d76-42bf-885a-58ccb4b05c28","isActive":false,"balance":"$3,756.96","picture":"http://placehold.it/32x32","age":21,"eyeColor":"blue","name":"Hester Pollard"},{"_id":"5b20b2e0fcc2dd1ced4cb4f0","index":4,"guid":"84be1331-cfd1-4cbd-a9b7-61d0ff47b48b","isActive":false,"balance":"$2,989.81","picture":"http://placehold.it/32x32","age":31,"eyeColor":"brown","name":"Terrell Dennis"},{"_id":"5b20b2e07cfa4624ef228d62","index":5,"guid":"38c86e8b-ec24-4a8c-a635-e9517e616c9a","isActive":true,"balance":"$3,195.17","picture":"http://placehold.it/32x32","age":30,"eyeColor":"blue","name":"Padilla Schultz"},{"_id":"5b20b2e0bc158c3a14dacf98","index":6,"guid":"c60a1b92-87df-4f28-87d7-3699d7219603","isActive":true,"balance":"$2,583.68","picture":"http://placehold.it/32x32","age":31,"eyeColor":"brown","name":"Marisol Brewer"}]</t>
-  </si>
-  <si>
-    <t>kokokoko</t>
-  </si>
-  <si>
-    <t>kkljlkjlkj</t>
-  </si>
-  <si>
-    <t>[{"_id":"5b20b333866cdbec105144f0","index":0,"guid":"fe4c40ba-1150-4ec7-be2b-68364b0ce1c3","isActive":true,"balance":"$1,557.90","picture":"http://placehold.it/32x32","age":29,"eyeColor":"brown","name":"Priscilla Townsend"},{"_id":"5b20b333f2b68773771fe88d","index":1,"guid":"ba7f3edf-f3db-46cf-9b68-cad0f26a159b","isActive":true,"balance":"$1,287.93","picture":"http://placehold.it/32x32","age":29,"eyeColor":"green","name":"Peggy Cherry"},{"_id":"5b20b333545e5f1a321976f6","index":2,"guid":"6f58410c-adb4-4ecd-87b3-59fd1dcbe936","isActive":false,"balance":"$2,818.10","picture":"http://placehold.it/32x32","age":38,"eyeColor":"brown","name":"Shepherd Barry"},{"_id":"5b20b333a66072a9828aba04","index":3,"guid":"774ddfc3-f81c-4e8d-a1bd-9fc3a1dbf6f9","isActive":true,"balance":"$3,666.68","picture":"http://placehold.it/32x32","age":24,"eyeColor":"blue","name":"Patton Hansen"},{"_id":"5b20b333a8ac10fa3032837c","index":4,"guid":"1f36bd52-18d8-46a7-a222-579ee34f0047","isActive":false,"balance":"$3,146.98","picture":"http://placehold.it/32x32","age":39,"eyeColor":"brown","name":"House Ross"}]</t>
-  </si>
-  <si>
-    <t>asdsoimas</t>
-  </si>
-  <si>
-    <t>[{"_id":"5b20b33d44b7ab485e26c63c","index":0,"guid":"70cd3fa3-715c-4b9c-adf0-055ac8224fb6","isActive":false,"balance":"$3,620.65","picture":"http://placehold.it/32x32","age":35,"eyeColor":"blue","name":"Vance Daniel"},{"_id":"5b20b33d5b49487ec4c8b9a8","index":1,"guid":"44464f93-900c-4baa-9be9-65bf83b34ff1","isActive":true,"balance":"$3,784.97","picture":"http://placehold.it/32x32","age":31,"eyeColor":"green","name":"Tania Preston"},{"_id":"5b20b33d2badf4414a697d92","index":2,"guid":"b4273a3e-0ed4-4522-a181-499307ce3169","isActive":true,"balance":"$1,365.76","picture":"http://placehold.it/32x32","age":24,"eyeColor":"brown","name":"Lea Whitehead"},{"_id":"5b20b33d8daddacd45035873","index":3,"guid":"422625a5-6f43-4701-ad85-308e315b1e2f","isActive":false,"balance":"$2,686.75","picture":"http://placehold.it/32x32","age":27,"eyeColor":"blue","name":"Rosemarie Duffy"},{"_id":"5b20b33d2ae9597c7b72050b","index":4,"guid":"9879a309-cae6-4df6-b174-a091bbcfe1f4","isActive":true,"balance":"$2,054.49","picture":"http://placehold.it/32x32","age":29,"eyeColor":"brown","name":"Richmond Kelly"},{"_id":"5b20b33df2a180bf70f6c60b","index":5,"guid":"15bda1b1-3664-4e56-8d5a-7e57fd09b28c","isActive":false,"balance":"$3,488.15","picture":"http://placehold.it/32x32","age":22,"eyeColor":"green","name":"Ware Farrell"}]</t>
-  </si>
-  <si>
-    <t>bhjjhbkj</t>
-  </si>
-  <si>
-    <t>[{"_id":"5b20b34e82d5cd0bd680ba1b","index":0,"guid":"79b38e4f-e01d-46e3-9056-d42d7f380d13","isActive":false,"balance":"$3,262.23","picture":"http://placehold.it/32x32","age":34,"eyeColor":"green","name":"Deena Christensen"},{"_id":"5b20b34ea7b98b8cf4cd0c20","index":1,"guid":"a7ddb384-2e70-431f-86e5-c230d9975ff6","isActive":true,"balance":"$1,771.32","picture":"http://placehold.it/32x32","age":25,"eyeColor":"green","name":"Buchanan Hansen"},{"_id":"5b20b34e33220c80a2c8c3cb","index":2,"guid":"7aa57696-b4b9-478d-b839-8da65de21d12","isActive":false,"balance":"$3,242.29","picture":"http://placehold.it/32x32","age":26,"eyeColor":"blue","name":"Terri Delgado"},{"_id":"5b20b34ef0157750358e1915","index":3,"guid":"b029c80f-cb38-4466-b57b-3a705bf3d23e","isActive":false,"balance":"$3,290.54","picture":"http://placehold.it/32x32","age":30,"eyeColor":"brown","name":"Erma Head"},{"_id":"5b20b34ebfdc19f86963a951","index":4,"guid":"ce546b89-aa0c-4ae5-b22f-4dff7eeec53c","isActive":true,"balance":"$1,627.31","picture":"http://placehold.it/32x32","age":21,"eyeColor":"brown","name":"Monica Noel"}]</t>
-  </si>
-  <si>
-    <t>asfkjsnadkj</t>
-  </si>
-  <si>
-    <t>[{"_id":"5b20b35662d2f811b90e3ea0","index":0,"guid":"b713538d-4335-407f-a6cc-30b0d6716f61","isActive":true,"balance":"$3,105.26","picture":"http://placehold.it/32x32","age":31,"eyeColor":"blue","name":"Socorro Zamora"},{"_id":"5b20b356b62f9569c207ca25","index":1,"guid":"12f48037-90ce-4a13-b06a-0d03852ac94b","isActive":false,"balance":"$1,055.62","picture":"http://placehold.it/32x32","age":40,"eyeColor":"blue","name":"Herring Poole"},{"_id":"5b20b356d3d7e856f31a9f4b","index":2,"guid":"1018f671-7e2f-4ff9-9764-bf7ae374d68e","isActive":true,"balance":"$2,106.42","picture":"http://placehold.it/32x32","age":27,"eyeColor":"green","name":"Hansen Trujillo"},{"_id":"5b20b356cf5c4e6c4f00e1e7","index":3,"guid":"0020a556-cdcb-4aed-8817-79a4e122e54f","isActive":false,"balance":"$3,791.11","picture":"http://placehold.it/32x32","age":38,"eyeColor":"blue","name":"Woodard Maldonado"},{"_id":"5b20b356c81d95f4c93fe0cb","index":4,"guid":"653902ba-9b28-4ff4-a0fb-9b44e9df0574","isActive":false,"balance":"$3,222.65","picture":"http://placehold.it/32x32","age":36,"eyeColor":"blue","name":"Phoebe Ramos"},{"_id":"5b20b35674e190d34f6134e7","index":5,"guid":"70cfc4db-1c3c-4595-a00e-71ae6295644c","isActive":false,"balance":"$1,336.14","picture":"http://placehold.it/32x32","age":33,"eyeColor":"green","name":"Fuentes Horn"},{"_id":"5b20b356d086c8ad6d838f08","index":6,"guid":"c832d343-20a3-402e-b41a-322eccc1fa15","isActive":false,"balance":"$3,190.74","picture":"http://placehold.it/32x32","age":21,"eyeColor":"blue","name":"Ramona Jimenez"}]</t>
+    <t>BooleanField</t>
   </si>
 </sst>
 </file>
@@ -413,118 +368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="n">
-        <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="n">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,27 +377,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B3" t="n">
-        <v>7</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -561,13 +389,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,62 +403,84 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="n">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="n">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added excel wrapper, made code more readable
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>NAME</t>
   </si>
@@ -81,45 +81,6 @@
   </si>
   <si>
     <t>asdkajsdasn</t>
-  </si>
-  <si>
-    <t>org2</t>
-  </si>
-  <si>
-    <t>desc2</t>
-  </si>
-  <si>
-    <t>temp1</t>
-  </si>
-  <si>
-    <t>kokokoko</t>
-  </si>
-  <si>
-    <t>conftemp1</t>
-  </si>
-  <si>
-    <t>asfkjsnadkj</t>
-  </si>
-  <si>
-    <t>org1</t>
-  </si>
-  <si>
-    <t>desc1</t>
-  </si>
-  <si>
-    <t>temp4</t>
-  </si>
-  <si>
-    <t>template</t>
-  </si>
-  <si>
-    <t>contemp4</t>
-  </si>
-  <si>
-    <t>multiselect</t>
-  </si>
-  <si>
-    <t>asdsfsafsa</t>
   </si>
 </sst>
 </file>
@@ -455,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,76 +529,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="n">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
better mechanism for retriving models fields and values
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>NAME</t>
   </si>
@@ -23,7 +23,13 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>TEMPLATE NAME</t>
+    <t>PROJECT_ID</t>
+  </si>
+  <si>
+    <t>SHEET</t>
+  </si>
+  <si>
+    <t>CONTENT_TYPE_ID</t>
   </si>
   <si>
     <t>OBJECT_ID</t>
@@ -32,15 +38,24 @@
     <t>TYPE</t>
   </si>
   <si>
+    <t>TEMPLATE_ID</t>
+  </si>
+  <si>
     <t>DB_FIELD</t>
   </si>
   <si>
     <t>DATA_TYPE</t>
   </si>
   <si>
+    <t>CONFIGURABLE_SETTING</t>
+  </si>
+  <si>
     <t>LABEL</t>
   </si>
   <si>
+    <t>EXCEPTIONS</t>
+  </si>
+  <si>
     <t>REQUIRED</t>
   </si>
   <si>
@@ -59,6 +74,9 @@
     <t>temp2</t>
   </si>
   <si>
+    <t>[{"_id":"5b20b297fc28b53b80bb588b","index":0,"guid":"b9cc2193-c475-4f86-9c5d-ba1c1eb17cfa","isActive":false,"balance":"$2,544.76","picture":"http://placehold.it/32x32","age":35,"eyeColor":"blue","name":"Deana Cohen"},{"_id":"5b20b2973f8a4a90ad8c35fc","index":1,"guid":"b2b0f4d5-39e1-4321-b300-3c08c0eacf4b","isActive":false,"balance":"$2,252.69","picture":"http://placehold.it/32x32","age":25,"eyeColor":"brown","name":"Chen Hooper"},{"_id":"5b20b2977df4355aa7b993af","index":2,"guid":"1f0c0829-f9ab-4eb6-b106-377e41086ddf","isActive":false,"balance":"$1,116.92","picture":"http://placehold.it/32x32","age":37,"eyeColor":"brown","name":"Arnold Wilson"},{"_id":"5b20b2973400739f91af8f3f","index":3,"guid":"14662d70-6e10-4d6b-bba8-24322fe79ad3","isActive":false,"balance":"$1,231.11","picture":"http://placehold.it/32x32","age":23,"eyeColor":"green","name":"Berta Clark"},{"_id":"5b20b297b9504bbe4b26303f","index":4,"guid":"966ec57f-f3ce-4eab-9d2f-636f3f1f89f1","isActive":true,"balance":"$1,310.59","picture":"http://placehold.it/32x32","age":35,"eyeColor":"brown","name":"Vaughn Ellison"},{"_id":"5b20b297f043757eca7cdedc","index":5,"guid":"22469496-b935-448a-b206-3fa34aa4341c","isActive":false,"balance":"$3,774.91","picture":"http://placehold.it/32x32","age":28,"eyeColor":"green","name":"Jacqueline Nixon"}]</t>
+  </si>
+  <si>
     <t>jojojojo</t>
   </si>
   <si>
@@ -68,16 +86,19 @@
     <t>int</t>
   </si>
   <si>
+    <t>[{"_id":"5b20b333866cdbec105144f0","index":0,"guid":"fe4c40ba-1150-4ec7-be2b-68364b0ce1c3","isActive":true,"balance":"$1,557.90","picture":"http://placehold.it/32x32","age":29,"eyeColor":"brown","name":"Priscilla Townsend"},{"_id":"5b20b333f2b68773771fe88d","index":1,"guid":"ba7f3edf-f3db-46cf-9b68-cad0f26a159b","isActive":true,"balance":"$1,287.93","picture":"http://placehold.it/32x32","age":29,"eyeColor":"green","name":"Peggy Cherry"},{"_id":"5b20b333545e5f1a321976f6","index":2,"guid":"6f58410c-adb4-4ecd-87b3-59fd1dcbe936","isActive":false,"balance":"$2,818.10","picture":"http://placehold.it/32x32","age":38,"eyeColor":"brown","name":"Shepherd Barry"},{"_id":"5b20b333a66072a9828aba04","index":3,"guid":"774ddfc3-f81c-4e8d-a1bd-9fc3a1dbf6f9","isActive":true,"balance":"$3,666.68","picture":"http://placehold.it/32x32","age":24,"eyeColor":"blue","name":"Patton Hansen"},{"_id":"5b20b333a8ac10fa3032837c","index":4,"guid":"1f36bd52-18d8-46a7-a222-579ee34f0047","isActive":false,"balance":"$3,146.98","picture":"http://placehold.it/32x32","age":39,"eyeColor":"brown","name":"House Ross"}]</t>
+  </si>
+  <si>
     <t>asdsoimas</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>True</t>
+    <t>[{"_id":"5b20b33d44b7ab485e26c63c","index":0,"guid":"70cd3fa3-715c-4b9c-adf0-055ac8224fb6","isActive":false,"balance":"$3,620.65","picture":"http://placehold.it/32x32","age":35,"eyeColor":"blue","name":"Vance Daniel"},{"_id":"5b20b33d5b49487ec4c8b9a8","index":1,"guid":"44464f93-900c-4baa-9be9-65bf83b34ff1","isActive":true,"balance":"$3,784.97","picture":"http://placehold.it/32x32","age":31,"eyeColor":"green","name":"Tania Preston"},{"_id":"5b20b33d2badf4414a697d92","index":2,"guid":"b4273a3e-0ed4-4522-a181-499307ce3169","isActive":true,"balance":"$1,365.76","picture":"http://placehold.it/32x32","age":24,"eyeColor":"brown","name":"Lea Whitehead"},{"_id":"5b20b33d8daddacd45035873","index":3,"guid":"422625a5-6f43-4701-ad85-308e315b1e2f","isActive":false,"balance":"$2,686.75","picture":"http://placehold.it/32x32","age":27,"eyeColor":"blue","name":"Rosemarie Duffy"},{"_id":"5b20b33d2ae9597c7b72050b","index":4,"guid":"9879a309-cae6-4df6-b174-a091bbcfe1f4","isActive":true,"balance":"$2,054.49","picture":"http://placehold.it/32x32","age":29,"eyeColor":"brown","name":"Richmond Kelly"},{"_id":"5b20b33df2a180bf70f6c60b","index":5,"guid":"15bda1b1-3664-4e56-8d5a-7e57fd09b28c","isActive":false,"balance":"$3,488.15","picture":"http://placehold.it/32x32","age":22,"eyeColor":"green","name":"Ware Farrell"}]</t>
   </si>
   <si>
     <t>table</t>
+  </si>
+  <si>
+    <t>[{"name":"Rodgers Delacruz","gender":"male","greeting":"Hello, Rodgers Delacruz! You have 10 unread messages.","favoriteFruit":"banana"},{"name":"Garcia Moon","gender":"male","greeting":"Hello, Garcia Moon! You have 5 unread messages.","favoriteFruit":"strawberry"},{"name":"Lane Patrick","gender":"male","greeting":"Hello, Lane Patrick! You have 3 unread messages.","favoriteFruit":"strawberry"},{"name":"Moody Barrera","gender":"male","greeting":"Hello, Moody Barrera! You have 7 unread messages.","favoriteFruit":"strawberry"},{"name":"Meagan Hester","gender":"female","greeting":"Hello, Meagan Hester! You have 3 unread messages.","favoriteFruit":"strawberry"},{"name":"Lewis Morse","gender":"male","greeting":"Hello, Lewis Morse! You have 3 unread messages.","favoriteFruit":"banana"},{"name":"Bonnie Cross","gender":"female","greeting":"Hello, Bonnie Cross! You have 1 unread messages.","favoriteFruit":"banana"}]</t>
   </si>
   <si>
     <t>asdkajsdasn</t>
@@ -416,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +445,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,101 +453,149 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="n">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="G3" t="n">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed method of accessing cell, fixed depreciated function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>PROJECT_ID</t>
+  </si>
+  <si>
+    <t>SHEET</t>
+  </si>
+  <si>
+    <t>CONTENT_TYPE_ID</t>
+  </si>
+  <si>
+    <t>OBJECT_ID</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>TEMPLATE_ID</t>
+  </si>
+  <si>
+    <t>DB_FIELD</t>
+  </si>
+  <si>
+    <t>DATA_TYPE</t>
+  </si>
+  <si>
+    <t>CONFIGURABLE_SETTING</t>
+  </si>
+  <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>EXCEPTIONS</t>
+  </si>
+  <si>
+    <t>REQUIRED</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>DISABLED</t>
+  </si>
+  <si>
+    <t>org3</t>
+  </si>
+  <si>
+    <t>desc3</t>
+  </si>
+  <si>
+    <t>temp2</t>
+  </si>
+  <si>
+    <t>[{"_id":"5b20b297fc28b53b80bb588b","index":0,"guid":"b9cc2193-c475-4f86-9c5d-ba1c1eb17cfa","isActive":false,"balance":"$2,544.76","picture":"http://placehold.it/32x32","age":35,"eyeColor":"blue","name":"Deana Cohen"},{"_id":"5b20b2973f8a4a90ad8c35fc","index":1,"guid":"b2b0f4d5-39e1-4321-b300-3c08c0eacf4b","isActive":false,"balance":"$2,252.69","picture":"http://placehold.it/32x32","age":25,"eyeColor":"brown","name":"Chen Hooper"},{"_id":"5b20b2977df4355aa7b993af","index":2,"guid":"1f0c0829-f9ab-4eb6-b106-377e41086ddf","isActive":false,"balance":"$1,116.92","picture":"http://placehold.it/32x32","age":37,"eyeColor":"brown","name":"Arnold Wilson"},{"_id":"5b20b2973400739f91af8f3f","index":3,"guid":"14662d70-6e10-4d6b-bba8-24322fe79ad3","isActive":false,"balance":"$1,231.11","picture":"http://placehold.it/32x32","age":23,"eyeColor":"green","name":"Berta Clark"},{"_id":"5b20b297b9504bbe4b26303f","index":4,"guid":"966ec57f-f3ce-4eab-9d2f-636f3f1f89f1","isActive":true,"balance":"$1,310.59","picture":"http://placehold.it/32x32","age":35,"eyeColor":"brown","name":"Vaughn Ellison"},{"_id":"5b20b297f043757eca7cdedc","index":5,"guid":"22469496-b935-448a-b206-3fa34aa4341c","isActive":false,"balance":"$3,774.91","picture":"http://placehold.it/32x32","age":28,"eyeColor":"green","name":"Jacqueline Nixon"}]</t>
+  </si>
+  <si>
+    <t>jojojojo</t>
+  </si>
+  <si>
+    <t>conftemp2</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>[{"_id":"5b20b333866cdbec105144f0","index":0,"guid":"fe4c40ba-1150-4ec7-be2b-68364b0ce1c3","isActive":true,"balance":"$1,557.90","picture":"http://placehold.it/32x32","age":29,"eyeColor":"brown","name":"Priscilla Townsend"},{"_id":"5b20b333f2b68773771fe88d","index":1,"guid":"ba7f3edf-f3db-46cf-9b68-cad0f26a159b","isActive":true,"balance":"$1,287.93","picture":"http://placehold.it/32x32","age":29,"eyeColor":"green","name":"Peggy Cherry"},{"_id":"5b20b333545e5f1a321976f6","index":2,"guid":"6f58410c-adb4-4ecd-87b3-59fd1dcbe936","isActive":false,"balance":"$2,818.10","picture":"http://placehold.it/32x32","age":38,"eyeColor":"brown","name":"Shepherd Barry"},{"_id":"5b20b333a66072a9828aba04","index":3,"guid":"774ddfc3-f81c-4e8d-a1bd-9fc3a1dbf6f9","isActive":true,"balance":"$3,666.68","picture":"http://placehold.it/32x32","age":24,"eyeColor":"blue","name":"Patton Hansen"},{"_id":"5b20b333a8ac10fa3032837c","index":4,"guid":"1f36bd52-18d8-46a7-a222-579ee34f0047","isActive":false,"balance":"$3,146.98","picture":"http://placehold.it/32x32","age":39,"eyeColor":"brown","name":"House Ross"}]</t>
+  </si>
+  <si>
+    <t>asdsoimas</t>
+  </si>
+  <si>
+    <t>[{"_id":"5b20b33d44b7ab485e26c63c","index":0,"guid":"70cd3fa3-715c-4b9c-adf0-055ac8224fb6","isActive":false,"balance":"$3,620.65","picture":"http://placehold.it/32x32","age":35,"eyeColor":"blue","name":"Vance Daniel"},{"_id":"5b20b33d5b49487ec4c8b9a8","index":1,"guid":"44464f93-900c-4baa-9be9-65bf83b34ff1","isActive":true,"balance":"$3,784.97","picture":"http://placehold.it/32x32","age":31,"eyeColor":"green","name":"Tania Preston"},{"_id":"5b20b33d2badf4414a697d92","index":2,"guid":"b4273a3e-0ed4-4522-a181-499307ce3169","isActive":true,"balance":"$1,365.76","picture":"http://placehold.it/32x32","age":24,"eyeColor":"brown","name":"Lea Whitehead"},{"_id":"5b20b33d8daddacd45035873","index":3,"guid":"422625a5-6f43-4701-ad85-308e315b1e2f","isActive":false,"balance":"$2,686.75","picture":"http://placehold.it/32x32","age":27,"eyeColor":"blue","name":"Rosemarie Duffy"},{"_id":"5b20b33d2ae9597c7b72050b","index":4,"guid":"9879a309-cae6-4df6-b174-a091bbcfe1f4","isActive":true,"balance":"$2,054.49","picture":"http://placehold.it/32x32","age":29,"eyeColor":"brown","name":"Richmond Kelly"},{"_id":"5b20b33df2a180bf70f6c60b","index":5,"guid":"15bda1b1-3664-4e56-8d5a-7e57fd09b28c","isActive":false,"balance":"$3,488.15","picture":"http://placehold.it/32x32","age":22,"eyeColor":"green","name":"Ware Farrell"}]</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>[{"name":"Rodgers Delacruz","gender":"male","greeting":"Hello, Rodgers Delacruz! You have 10 unread messages.","favoriteFruit":"banana"},{"name":"Garcia Moon","gender":"male","greeting":"Hello, Garcia Moon! You have 5 unread messages.","favoriteFruit":"strawberry"},{"name":"Lane Patrick","gender":"male","greeting":"Hello, Lane Patrick! You have 3 unread messages.","favoriteFruit":"strawberry"},{"name":"Moody Barrera","gender":"male","greeting":"Hello, Moody Barrera! You have 7 unread messages.","favoriteFruit":"strawberry"},{"name":"Meagan Hester","gender":"female","greeting":"Hello, Meagan Hester! You have 3 unread messages.","favoriteFruit":"strawberry"},{"name":"Lewis Morse","gender":"male","greeting":"Hello, Lewis Morse! You have 3 unread messages.","favoriteFruit":"banana"},{"name":"Bonnie Cross","gender":"female","greeting":"Hello, Bonnie Cross! You have 1 unread messages.","favoriteFruit":"banana"}]</t>
+  </si>
+  <si>
+    <t>asdkajsdasn</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -388,7 +476,161 @@
   <cols>
     <col customWidth="1" max="1025" min="1" style="1" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="n">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="n">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="1" verticalDpi="300"/>

</xml_diff>